<commit_message>
Ready POO, felicidades a los que pasaron lastima por los que se quedaron
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/_POO (Autosaved).xlsx
+++ b/OYM/_DocumentosComunes/_POO (Autosaved).xlsx
@@ -15,7 +15,7 @@
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$90</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -1146,8 +1146,8 @@
   <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M81" sqref="M81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M90" sqref="M90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1276,20 +1276,20 @@
         <v>17</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D66" si="0">IF((N3)&gt;=70,10,"")</f>
+        <f>IF((N3)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E66" si="1">IF((N3)&gt;=70,20,"")</f>
+        <f>IF((N3)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F66" si="2">IF((N3)&gt;=70,20,"")</f>
+        <f>IF((N3)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G66" si="3">IF((N3)&gt;=70,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
-        <v>29</v>
+        <f>IF((N3)&gt;=70,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -1304,11 +1304,11 @@
         <v>20</v>
       </c>
       <c r="M3">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N66" si="4">IF((H3+I3+J3+L3+M3+O3)&lt;70,IF((H3+I3+J3+L3+M3+O3)&gt;59,70,(H3+I3+J3+L3+M3+O3)),(H3+I3+J3+L3+M3+O3))</f>
-        <v>79</v>
+        <f>IF((H3+I3+J3+L3+M3+O3)&lt;70,IF((H3+I3+J3+L3+M3+O3)&gt;59,70,(H3+I3+J3+L3+M3+O3)),(H3+I3+J3+L3+M3+O3))</f>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1322,26 +1322,26 @@
         <v>19</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N4)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E4" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N4)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F4" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N4)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G4" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N4)&gt;=70,IF((N4-50)&gt;50,50,IF((N4-50)&lt;0,0,(N4-50))), "" )</f>
         <v/>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="N4">
-        <f t="shared" si="4"/>
+        <f>IF((H4+I4+J4+L4+M4+O4)&lt;70,IF((H4+I4+J4+L4+M4+O4)&gt;59,70,(H4+I4+J4+L4+M4+O4)),(H4+I4+J4+L4+M4+O4))</f>
         <v>0</v>
       </c>
     </row>
@@ -1355,21 +1355,21 @@
       <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F5" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G5" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D5" s="6">
+        <f>IF((N5)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E5" s="2">
+        <f>IF((N5)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F5" s="2">
+        <f>IF((N5)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G5" s="6">
+        <f>IF((N5)&gt;=70,IF((N5-50)&gt;50,50,IF((N5-50)&lt;0,0,(N5-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="J5">
         <v>14</v>
@@ -1380,9 +1380,12 @@
       <c r="L5">
         <v>18</v>
       </c>
+      <c r="M5">
+        <v>28</v>
+      </c>
       <c r="N5">
-        <f t="shared" si="4"/>
-        <v>32</v>
+        <f>IF((H5+I5+J5+L5+M5+O5)&lt;70,IF((H5+I5+J5+L5+M5+O5)&gt;59,70,(H5+I5+J5+L5+M5+O5)),(H5+I5+J5+L5+M5+O5))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1396,19 +1399,19 @@
         <v>23</v>
       </c>
       <c r="D6" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N6)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N6)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N6)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G6" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N6)&gt;=70,IF((N6-50)&gt;50,50,IF((N6-50)&lt;0,0,(N6-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H6">
@@ -1427,7 +1430,7 @@
         <v>26</v>
       </c>
       <c r="N6">
-        <f t="shared" si="4"/>
+        <f>IF((H6+I6+J6+L6+M6+O6)&lt;70,IF((H6+I6+J6+L6+M6+O6)&gt;59,70,(H6+I6+J6+L6+M6+O6)),(H6+I6+J6+L6+M6+O6))</f>
         <v>70</v>
       </c>
     </row>
@@ -1442,19 +1445,19 @@
         <v>25</v>
       </c>
       <c r="D7" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N7)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N7)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F7" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N7)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G7" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N7)&gt;=70,IF((N7-50)&gt;50,50,IF((N7-50)&lt;0,0,(N7-50))), "" )</f>
         <v/>
       </c>
       <c r="H7">
@@ -1467,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="4"/>
+        <f>IF((H7+I7+J7+L7+M7+O7)&lt;70,IF((H7+I7+J7+L7+M7+O7)&gt;59,70,(H7+I7+J7+L7+M7+O7)),(H7+I7+J7+L7+M7+O7))</f>
         <v>12</v>
       </c>
     </row>
@@ -1482,20 +1485,20 @@
         <v>27</v>
       </c>
       <c r="D8" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N8)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N8)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N8)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N8)&gt;=70,IF((N8-50)&gt;50,50,IF((N8-50)&lt;0,0,(N8-50))), "" )</f>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>20</v>
@@ -1512,9 +1515,12 @@
       <c r="L8">
         <v>20</v>
       </c>
+      <c r="M8">
+        <v>28</v>
+      </c>
       <c r="N8">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H8+I8+J8+L8+M8+O8)&lt;70,IF((H8+I8+J8+L8+M8+O8)&gt;59,70,(H8+I8+J8+L8+M8+O8)),(H8+I8+J8+L8+M8+O8))</f>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1528,19 +1534,19 @@
         <v>29</v>
       </c>
       <c r="D9" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N9)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N9)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N9)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N9)&gt;=70,IF((N9-50)&gt;50,50,IF((N9-50)&lt;0,0,(N9-50))), "" )</f>
         <v>28</v>
       </c>
       <c r="H9">
@@ -1559,7 +1565,7 @@
         <v>28</v>
       </c>
       <c r="N9">
-        <f t="shared" si="4"/>
+        <f>IF((H9+I9+J9+L9+M9+O9)&lt;70,IF((H9+I9+J9+L9+M9+O9)&gt;59,70,(H9+I9+J9+L9+M9+O9)),(H9+I9+J9+L9+M9+O9))</f>
         <v>78</v>
       </c>
     </row>
@@ -1574,19 +1580,19 @@
         <v>31</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N10)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N10)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N10)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N10)&gt;=70,IF((N10-50)&gt;50,50,IF((N10-50)&lt;0,0,(N10-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H10">
@@ -1605,7 +1611,7 @@
         <v>21</v>
       </c>
       <c r="N10">
-        <f t="shared" si="4"/>
+        <f>IF((H10+I10+J10+L10+M10+O10)&lt;70,IF((H10+I10+J10+L10+M10+O10)&gt;59,70,(H10+I10+J10+L10+M10+O10)),(H10+I10+J10+L10+M10+O10))</f>
         <v>70</v>
       </c>
     </row>
@@ -1620,19 +1626,19 @@
         <v>33</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N11)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N11)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N11)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N11)&gt;=70,IF((N11-50)&gt;50,50,IF((N11-50)&lt;0,0,(N11-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H11">
@@ -1651,7 +1657,7 @@
         <v>20</v>
       </c>
       <c r="N11">
-        <f t="shared" si="4"/>
+        <f>IF((H11+I11+J11+L11+M11+O11)&lt;70,IF((H11+I11+J11+L11+M11+O11)&gt;59,70,(H11+I11+J11+L11+M11+O11)),(H11+I11+J11+L11+M11+O11))</f>
         <v>70</v>
       </c>
     </row>
@@ -1665,21 +1671,21 @@
       <c r="C12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F12" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G12" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D12" s="6">
+        <f>IF((N12)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E12" s="2">
+        <f>IF((N12)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F12" s="2">
+        <f>IF((N12)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G12" s="6">
+        <f>IF((N12)&gt;=70,IF((N12-50)&gt;50,50,IF((N12-50)&lt;0,0,(N12-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H12">
         <v>20</v>
@@ -1690,9 +1696,12 @@
       <c r="K12">
         <v>1</v>
       </c>
+      <c r="M12">
+        <v>28</v>
+      </c>
       <c r="N12">
-        <f t="shared" si="4"/>
-        <v>33</v>
+        <f>IF((H12+I12+J12+L12+M12+O12)&lt;70,IF((H12+I12+J12+L12+M12+O12)&gt;59,70,(H12+I12+J12+L12+M12+O12)),(H12+I12+J12+L12+M12+O12))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1705,21 +1714,21 @@
       <c r="C13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G13" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D13" s="6">
+        <f>IF((N13)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <f>IF((N13)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F13" s="2">
+        <f>IF((N13)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G13" s="6">
+        <f>IF((N13)&gt;=70,IF((N13-50)&gt;50,50,IF((N13-50)&lt;0,0,(N13-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="I13">
         <v>10</v>
@@ -1733,9 +1742,12 @@
       <c r="L13">
         <v>20</v>
       </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
       <c r="N13">
-        <f t="shared" si="4"/>
-        <v>48</v>
+        <f>IF((H13+I13+J13+L13+M13+O13)&lt;70,IF((H13+I13+J13+L13+M13+O13)&gt;59,70,(H13+I13+J13+L13+M13+O13)),(H13+I13+J13+L13+M13+O13))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1748,21 +1760,21 @@
       <c r="C14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E14" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G14" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D14" s="6">
+        <f>IF((N14)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
+        <f>IF((N14)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F14" s="2">
+        <f>IF((N14)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G14" s="6">
+        <f>IF((N14)&gt;=70,IF((N14-50)&gt;50,50,IF((N14-50)&lt;0,0,(N14-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H14">
         <v>12</v>
@@ -1773,9 +1785,12 @@
       <c r="L14">
         <v>20</v>
       </c>
+      <c r="M14">
+        <v>28</v>
+      </c>
       <c r="N14">
-        <f t="shared" si="4"/>
-        <v>32</v>
+        <f>IF((H14+I14+J14+L14+M14+O14)&lt;70,IF((H14+I14+J14+L14+M14+O14)&gt;59,70,(H14+I14+J14+L14+M14+O14)),(H14+I14+J14+L14+M14+O14))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1789,19 +1804,19 @@
         <v>41</v>
       </c>
       <c r="D15" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N15)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N15)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F15" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N15)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G15" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N15)&gt;=70,IF((N15-50)&gt;50,50,IF((N15-50)&lt;0,0,(N15-50))), "" )</f>
         <v/>
       </c>
       <c r="H15">
@@ -1820,7 +1835,7 @@
         <v>20</v>
       </c>
       <c r="N15">
-        <f t="shared" si="4"/>
+        <f>IF((H15+I15+J15+L15+M15+O15)&lt;70,IF((H15+I15+J15+L15+M15+O15)&gt;59,70,(H15+I15+J15+L15+M15+O15)),(H15+I15+J15+L15+M15+O15))</f>
         <v>57</v>
       </c>
     </row>
@@ -1835,20 +1850,20 @@
         <v>43</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N16)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N16)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N16)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N16)&gt;=70,IF((N16-50)&gt;50,50,IF((N16-50)&lt;0,0,(N16-50))), "" )</f>
+        <v>41</v>
       </c>
       <c r="H16">
         <v>18</v>
@@ -1865,9 +1880,12 @@
       <c r="L16">
         <v>15</v>
       </c>
+      <c r="M16">
+        <v>30</v>
+      </c>
       <c r="N16">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H16+I16+J16+L16+M16+O16)&lt;70,IF((H16+I16+J16+L16+M16+O16)&gt;59,70,(H16+I16+J16+L16+M16+O16)),(H16+I16+J16+L16+M16+O16))</f>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1881,26 +1899,26 @@
         <v>45</v>
       </c>
       <c r="D17" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N17)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N17)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F17" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N17)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G17" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N17)&gt;=70,IF((N17-50)&gt;50,50,IF((N17-50)&lt;0,0,(N17-50))), "" )</f>
         <v/>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="N17">
-        <f t="shared" si="4"/>
+        <f>IF((H17+I17+J17+L17+M17+O17)&lt;70,IF((H17+I17+J17+L17+M17+O17)&gt;59,70,(H17+I17+J17+L17+M17+O17)),(H17+I17+J17+L17+M17+O17))</f>
         <v>0</v>
       </c>
     </row>
@@ -1915,19 +1933,19 @@
         <v>47</v>
       </c>
       <c r="D18" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N18)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N18)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F18" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N18)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G18" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N18)&gt;=70,IF((N18-50)&gt;50,50,IF((N18-50)&lt;0,0,(N18-50))), "" )</f>
         <v/>
       </c>
       <c r="I18">
@@ -1937,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="N18">
-        <f t="shared" si="4"/>
+        <f>IF((H18+I18+J18+L18+M18+O18)&lt;70,IF((H18+I18+J18+L18+M18+O18)&gt;59,70,(H18+I18+J18+L18+M18+O18)),(H18+I18+J18+L18+M18+O18))</f>
         <v>10</v>
       </c>
     </row>
@@ -1952,26 +1970,26 @@
         <v>49</v>
       </c>
       <c r="D19" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N19)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N19)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F19" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N19)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G19" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N19)&gt;=70,IF((N19-50)&gt;50,50,IF((N19-50)&lt;0,0,(N19-50))), "" )</f>
         <v/>
       </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="N19">
-        <f t="shared" si="4"/>
+        <f>IF((H19+I19+J19+L19+M19+O19)&lt;70,IF((H19+I19+J19+L19+M19+O19)&gt;59,70,(H19+I19+J19+L19+M19+O19)),(H19+I19+J19+L19+M19+O19))</f>
         <v>0</v>
       </c>
     </row>
@@ -1986,20 +2004,20 @@
         <v>51</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N20)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N20)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N20)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N20)&gt;=70,IF((N20-50)&gt;50,50,IF((N20-50)&lt;0,0,(N20-50))), "" )</f>
+        <v>41</v>
       </c>
       <c r="H20">
         <v>16</v>
@@ -2016,9 +2034,12 @@
       <c r="L20">
         <v>18</v>
       </c>
+      <c r="M20">
+        <v>30</v>
+      </c>
       <c r="N20">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H20+I20+J20+L20+M20+O20)&lt;70,IF((H20+I20+J20+L20+M20+O20)&gt;59,70,(H20+I20+J20+L20+M20+O20)),(H20+I20+J20+L20+M20+O20))</f>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2032,19 +2053,19 @@
         <v>53</v>
       </c>
       <c r="D21" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N21)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N21)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N21)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N21)&gt;=70,IF((N21-50)&gt;50,50,IF((N21-50)&lt;0,0,(N21-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="I21">
@@ -2063,7 +2084,7 @@
         <v>30</v>
       </c>
       <c r="N21">
-        <f t="shared" si="4"/>
+        <f>IF((H21+I21+J21+L21+M21+O21)&lt;70,IF((H21+I21+J21+L21+M21+O21)&gt;59,70,(H21+I21+J21+L21+M21+O21)),(H21+I21+J21+L21+M21+O21))</f>
         <v>70</v>
       </c>
     </row>
@@ -2077,21 +2098,21 @@
       <c r="C22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E22" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G22" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D22" s="6">
+        <f>IF((N22)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E22" s="2">
+        <f>IF((N22)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F22" s="2">
+        <f>IF((N22)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G22" s="6">
+        <f>IF((N22)&gt;=70,IF((N22-50)&gt;50,50,IF((N22-50)&lt;0,0,(N22-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H22">
         <v>18</v>
@@ -2105,9 +2126,12 @@
       <c r="L22">
         <v>18</v>
       </c>
+      <c r="M22">
+        <v>14</v>
+      </c>
       <c r="N22">
-        <f t="shared" si="4"/>
-        <v>46</v>
+        <f>IF((H22+I22+J22+L22+M22+O22)&lt;70,IF((H22+I22+J22+L22+M22+O22)&gt;59,70,(H22+I22+J22+L22+M22+O22)),(H22+I22+J22+L22+M22+O22))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2121,20 +2145,20 @@
         <v>57</v>
       </c>
       <c r="D23" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N23)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N23)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N23)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N23)&gt;=70,IF((N23-50)&gt;50,50,IF((N23-50)&lt;0,0,(N23-50))), "" )</f>
+        <v>46</v>
       </c>
       <c r="H23">
         <v>20</v>
@@ -2151,9 +2175,12 @@
       <c r="L23">
         <v>20</v>
       </c>
+      <c r="M23">
+        <v>28</v>
+      </c>
       <c r="N23">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H23+I23+J23+L23+M23+O23)&lt;70,IF((H23+I23+J23+L23+M23+O23)&gt;59,70,(H23+I23+J23+L23+M23+O23)),(H23+I23+J23+L23+M23+O23))</f>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2167,26 +2194,26 @@
         <v>59</v>
       </c>
       <c r="D24" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N24)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N24)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N24)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G24" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N24)&gt;=70,IF((N24-50)&gt;50,50,IF((N24-50)&lt;0,0,(N24-50))), "" )</f>
         <v/>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="N24">
-        <f t="shared" si="4"/>
+        <f>IF((H24+I24+J24+L24+M24+O24)&lt;70,IF((H24+I24+J24+L24+M24+O24)&gt;59,70,(H24+I24+J24+L24+M24+O24)),(H24+I24+J24+L24+M24+O24))</f>
         <v>0</v>
       </c>
     </row>
@@ -2201,19 +2228,19 @@
         <v>61</v>
       </c>
       <c r="D25" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N25)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N25)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F25" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N25)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G25" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N25)&gt;=70,IF((N25-50)&gt;50,50,IF((N25-50)&lt;0,0,(N25-50))), "" )</f>
         <v/>
       </c>
       <c r="J25">
@@ -2223,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="4"/>
+        <f>IF((H25+I25+J25+L25+M25+O25)&lt;70,IF((H25+I25+J25+L25+M25+O25)&gt;59,70,(H25+I25+J25+L25+M25+O25)),(H25+I25+J25+L25+M25+O25))</f>
         <v>15</v>
       </c>
     </row>
@@ -2238,20 +2265,20 @@
         <v>63</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N26)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N26)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N26)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G26" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N26)&gt;=70,IF((N26-50)&gt;50,50,IF((N26-50)&lt;0,0,(N26-50))), "" )</f>
+        <v>38</v>
       </c>
       <c r="H26">
         <v>20</v>
@@ -2265,9 +2292,12 @@
       <c r="L26">
         <v>20</v>
       </c>
+      <c r="M26">
+        <v>28</v>
+      </c>
       <c r="N26">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H26+I26+J26+L26+M26+O26)&lt;70,IF((H26+I26+J26+L26+M26+O26)&gt;59,70,(H26+I26+J26+L26+M26+O26)),(H26+I26+J26+L26+M26+O26))</f>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2281,19 +2311,19 @@
         <v>65</v>
       </c>
       <c r="D27" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N27)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N27)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F27" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N27)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G27" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N27)&gt;=70,IF((N27-50)&gt;50,50,IF((N27-50)&lt;0,0,(N27-50))), "" )</f>
         <v/>
       </c>
       <c r="I27">
@@ -2306,7 +2336,7 @@
         <v>14</v>
       </c>
       <c r="N27">
-        <f t="shared" si="4"/>
+        <f>IF((H27+I27+J27+L27+M27+O27)&lt;70,IF((H27+I27+J27+L27+M27+O27)&gt;59,70,(H27+I27+J27+L27+M27+O27)),(H27+I27+J27+L27+M27+O27))</f>
         <v>24</v>
       </c>
     </row>
@@ -2321,20 +2351,20 @@
         <v>67</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N28)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N28)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N28)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G28" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N28)&gt;=70,IF((N28-50)&gt;50,50,IF((N28-50)&lt;0,0,(N28-50))), "" )</f>
+        <v>40</v>
       </c>
       <c r="H28">
         <v>20</v>
@@ -2351,9 +2381,12 @@
       <c r="L28">
         <v>16</v>
       </c>
+      <c r="M28">
+        <v>28</v>
+      </c>
       <c r="N28">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H28+I28+J28+L28+M28+O28)&lt;70,IF((H28+I28+J28+L28+M28+O28)&gt;59,70,(H28+I28+J28+L28+M28+O28)),(H28+I28+J28+L28+M28+O28))</f>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2366,21 +2399,21 @@
       <c r="C29" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E29" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G29" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D29" s="6">
+        <f>IF((N29)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <f>IF((N29)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F29" s="2">
+        <f>IF((N29)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G29" s="6">
+        <f>IF((N29)&gt;=70,IF((N29-50)&gt;50,50,IF((N29-50)&lt;0,0,(N29-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H29">
         <v>15</v>
@@ -2394,9 +2427,12 @@
       <c r="L29">
         <v>20</v>
       </c>
+      <c r="M29">
+        <v>25</v>
+      </c>
       <c r="N29">
-        <f t="shared" si="4"/>
-        <v>35</v>
+        <f>IF((H29+I29+J29+L29+M29+O29)&lt;70,IF((H29+I29+J29+L29+M29+O29)&gt;59,70,(H29+I29+J29+L29+M29+O29)),(H29+I29+J29+L29+M29+O29))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2409,21 +2445,21 @@
       <c r="C30" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E30" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F30" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G30" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D30" s="6">
+        <f>IF((N30)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E30" s="2">
+        <f>IF((N30)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F30" s="2">
+        <f>IF((N30)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G30" s="6">
+        <f>IF((N30)&gt;=70,IF((N30-50)&gt;50,50,IF((N30-50)&lt;0,0,(N30-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="I30">
         <v>10</v>
@@ -2437,9 +2473,12 @@
       <c r="L30">
         <v>18</v>
       </c>
+      <c r="M30">
+        <v>16</v>
+      </c>
       <c r="N30">
-        <f t="shared" si="4"/>
-        <v>44</v>
+        <f>IF((H30+I30+J30+L30+M30+O30)&lt;70,IF((H30+I30+J30+L30+M30+O30)&gt;59,70,(H30+I30+J30+L30+M30+O30)),(H30+I30+J30+L30+M30+O30))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2453,19 +2492,19 @@
         <v>73</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N31)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N31)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N31)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G31" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N31)&gt;=70,IF((N31-50)&gt;50,50,IF((N31-50)&lt;0,0,(N31-50))), "" )</f>
         <v>21</v>
       </c>
       <c r="H31">
@@ -2484,7 +2523,7 @@
         <v>21</v>
       </c>
       <c r="N31">
-        <f t="shared" si="4"/>
+        <f>IF((H31+I31+J31+L31+M31+O31)&lt;70,IF((H31+I31+J31+L31+M31+O31)&gt;59,70,(H31+I31+J31+L31+M31+O31)),(H31+I31+J31+L31+M31+O31))</f>
         <v>71</v>
       </c>
     </row>
@@ -2499,19 +2538,19 @@
         <v>75</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N32)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N32)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N32)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G32" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N32)&gt;=70,IF((N32-50)&gt;50,50,IF((N32-50)&lt;0,0,(N32-50))), "" )</f>
         <v>29</v>
       </c>
       <c r="H32">
@@ -2530,7 +2569,7 @@
         <v>28</v>
       </c>
       <c r="N32">
-        <f t="shared" si="4"/>
+        <f>IF((H32+I32+J32+L32+M32+O32)&lt;70,IF((H32+I32+J32+L32+M32+O32)&gt;59,70,(H32+I32+J32+L32+M32+O32)),(H32+I32+J32+L32+M32+O32))</f>
         <v>79</v>
       </c>
     </row>
@@ -2545,19 +2584,19 @@
         <v>77</v>
       </c>
       <c r="D33" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N33)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N33)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N33)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G33" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N33)&gt;=70,IF((N33-50)&gt;50,50,IF((N33-50)&lt;0,0,(N33-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H33">
@@ -2573,7 +2612,7 @@
         <v>28</v>
       </c>
       <c r="N33">
-        <f t="shared" si="4"/>
+        <f>IF((H33+I33+J33+L33+M33+O33)&lt;70,IF((H33+I33+J33+L33+M33+O33)&gt;59,70,(H33+I33+J33+L33+M33+O33)),(H33+I33+J33+L33+M33+O33))</f>
         <v>70</v>
       </c>
     </row>
@@ -2588,19 +2627,19 @@
         <v>79</v>
       </c>
       <c r="D34" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N34)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E34" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N34)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N34)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G34" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N34)&gt;=70,IF((N34-50)&gt;50,50,IF((N34-50)&lt;0,0,(N34-50))), "" )</f>
         <v/>
       </c>
       <c r="H34">
@@ -2616,7 +2655,7 @@
         <v>18</v>
       </c>
       <c r="N34">
-        <f t="shared" si="4"/>
+        <f>IF((H34+I34+J34+L34+M34+O34)&lt;70,IF((H34+I34+J34+L34+M34+O34)&gt;59,70,(H34+I34+J34+L34+M34+O34)),(H34+I34+J34+L34+M34+O34))</f>
         <v>50</v>
       </c>
     </row>
@@ -2631,19 +2670,19 @@
         <v>81</v>
       </c>
       <c r="D35" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N35)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E35" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N35)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F35" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N35)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G35" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N35)&gt;=70,IF((N35-50)&gt;50,50,IF((N35-50)&lt;0,0,(N35-50))), "" )</f>
         <v/>
       </c>
       <c r="H35">
@@ -2659,7 +2698,7 @@
         <v>15</v>
       </c>
       <c r="N35">
-        <f t="shared" si="4"/>
+        <f>IF((H35+I35+J35+L35+M35+O35)&lt;70,IF((H35+I35+J35+L35+M35+O35)&gt;59,70,(H35+I35+J35+L35+M35+O35)),(H35+I35+J35+L35+M35+O35))</f>
         <v>40</v>
       </c>
     </row>
@@ -2674,19 +2713,19 @@
         <v>83</v>
       </c>
       <c r="D36" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N36)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E36" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N36)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F36" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N36)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G36" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N36)&gt;=70,IF((N36-50)&gt;50,50,IF((N36-50)&lt;0,0,(N36-50))), "" )</f>
         <v/>
       </c>
       <c r="H36">
@@ -2699,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <f t="shared" si="4"/>
+        <f>IF((H36+I36+J36+L36+M36+O36)&lt;70,IF((H36+I36+J36+L36+M36+O36)&gt;59,70,(H36+I36+J36+L36+M36+O36)),(H36+I36+J36+L36+M36+O36))</f>
         <v>37</v>
       </c>
     </row>
@@ -2714,19 +2753,19 @@
         <v>85</v>
       </c>
       <c r="D37" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N37)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N37)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N37)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G37" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N37)&gt;=70,IF((N37-50)&gt;50,50,IF((N37-50)&lt;0,0,(N37-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="J37">
@@ -2742,7 +2781,7 @@
         <v>27</v>
       </c>
       <c r="N37">
-        <f t="shared" si="4"/>
+        <f>IF((H37+I37+J37+L37+M37+O37)&lt;70,IF((H37+I37+J37+L37+M37+O37)&gt;59,70,(H37+I37+J37+L37+M37+O37)),(H37+I37+J37+L37+M37+O37))</f>
         <v>70</v>
       </c>
     </row>
@@ -2757,19 +2796,19 @@
         <v>87</v>
       </c>
       <c r="D38" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N38)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E38" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N38)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F38" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N38)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G38" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N38)&gt;=70,IF((N38-50)&gt;50,50,IF((N38-50)&lt;0,0,(N38-50))), "" )</f>
         <v/>
       </c>
       <c r="H38">
@@ -2782,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="N38">
-        <f t="shared" si="4"/>
+        <f>IF((H38+I38+J38+L38+M38+O38)&lt;70,IF((H38+I38+J38+L38+M38+O38)&gt;59,70,(H38+I38+J38+L38+M38+O38)),(H38+I38+J38+L38+M38+O38))</f>
         <v>33</v>
       </c>
     </row>
@@ -2797,19 +2836,19 @@
         <v>89</v>
       </c>
       <c r="D39" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N39)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E39" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N39)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F39" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N39)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G39" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N39)&gt;=70,IF((N39-50)&gt;50,50,IF((N39-50)&lt;0,0,(N39-50))), "" )</f>
         <v/>
       </c>
       <c r="H39">
@@ -2825,7 +2864,7 @@
         <v>21</v>
       </c>
       <c r="N39">
-        <f t="shared" si="4"/>
+        <f>IF((H39+I39+J39+L39+M39+O39)&lt;70,IF((H39+I39+J39+L39+M39+O39)&gt;59,70,(H39+I39+J39+L39+M39+O39)),(H39+I39+J39+L39+M39+O39))</f>
         <v>58</v>
       </c>
     </row>
@@ -2840,20 +2879,20 @@
         <v>91</v>
       </c>
       <c r="D40" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N40)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N40)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N40)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N40)&gt;=70,IF((N40-50)&gt;50,50,IF((N40-50)&lt;0,0,(N40-50))), "" )</f>
+        <v>30</v>
       </c>
       <c r="H40">
         <v>16</v>
@@ -2870,9 +2909,12 @@
       <c r="L40">
         <v>18</v>
       </c>
+      <c r="M40">
+        <v>20</v>
+      </c>
       <c r="N40">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H40+I40+J40+L40+M40+O40)&lt;70,IF((H40+I40+J40+L40+M40+O40)&gt;59,70,(H40+I40+J40+L40+M40+O40)),(H40+I40+J40+L40+M40+O40))</f>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2886,19 +2928,19 @@
         <v>93</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N41)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N41)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N41)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N41)&gt;=70,IF((N41-50)&gt;50,50,IF((N41-50)&lt;0,0,(N41-50))), "" )</f>
         <v>36</v>
       </c>
       <c r="H41">
@@ -2917,7 +2959,7 @@
         <v>30</v>
       </c>
       <c r="N41">
-        <f t="shared" si="4"/>
+        <f>IF((H41+I41+J41+L41+M41+O41)&lt;70,IF((H41+I41+J41+L41+M41+O41)&gt;59,70,(H41+I41+J41+L41+M41+O41)),(H41+I41+J41+L41+M41+O41))</f>
         <v>86</v>
       </c>
     </row>
@@ -2932,19 +2974,19 @@
         <v>95</v>
       </c>
       <c r="D42" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N42)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E42" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N42)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F42" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N42)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G42" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N42)&gt;=70,IF((N42-50)&gt;50,50,IF((N42-50)&lt;0,0,(N42-50))), "" )</f>
         <v/>
       </c>
       <c r="H42">
@@ -2960,7 +3002,7 @@
         <v>1</v>
       </c>
       <c r="N42">
-        <f t="shared" si="4"/>
+        <f>IF((H42+I42+J42+L42+M42+O42)&lt;70,IF((H42+I42+J42+L42+M42+O42)&gt;59,70,(H42+I42+J42+L42+M42+O42)),(H42+I42+J42+L42+M42+O42))</f>
         <v>40</v>
       </c>
     </row>
@@ -2975,19 +3017,19 @@
         <v>97</v>
       </c>
       <c r="D43" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N43)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N43)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N43)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G43" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N43)&gt;=70,IF((N43-50)&gt;50,50,IF((N43-50)&lt;0,0,(N43-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H43">
@@ -3006,7 +3048,7 @@
         <v>18</v>
       </c>
       <c r="N43">
-        <f t="shared" si="4"/>
+        <f>IF((H43+I43+J43+L43+M43+O43)&lt;70,IF((H43+I43+J43+L43+M43+O43)&gt;59,70,(H43+I43+J43+L43+M43+O43)),(H43+I43+J43+L43+M43+O43))</f>
         <v>70</v>
       </c>
     </row>
@@ -3021,20 +3063,20 @@
         <v>99</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N44)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N44)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N44)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N44)&gt;=70,IF((N44-50)&gt;50,50,IF((N44-50)&lt;0,0,(N44-50))), "" )</f>
+        <v>41</v>
       </c>
       <c r="H44">
         <v>20</v>
@@ -3051,9 +3093,12 @@
       <c r="L44">
         <v>17</v>
       </c>
+      <c r="M44">
+        <v>28</v>
+      </c>
       <c r="N44">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H44+I44+J44+L44+M44+O44)&lt;70,IF((H44+I44+J44+L44+M44+O44)&gt;59,70,(H44+I44+J44+L44+M44+O44)),(H44+I44+J44+L44+M44+O44))</f>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3067,26 +3112,26 @@
         <v>101</v>
       </c>
       <c r="D45" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N45)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E45" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N45)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F45" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N45)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G45" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N45)&gt;=70,IF((N45-50)&gt;50,50,IF((N45-50)&lt;0,0,(N45-50))), "" )</f>
         <v/>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="N45">
-        <f t="shared" si="4"/>
+        <f>IF((H45+I45+J45+L45+M45+O45)&lt;70,IF((H45+I45+J45+L45+M45+O45)&gt;59,70,(H45+I45+J45+L45+M45+O45)),(H45+I45+J45+L45+M45+O45))</f>
         <v>0</v>
       </c>
     </row>
@@ -3101,19 +3146,19 @@
         <v>103</v>
       </c>
       <c r="D46" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N46)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E46" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N46)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F46" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N46)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G46" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N46)&gt;=70,IF((N46-50)&gt;50,50,IF((N46-50)&lt;0,0,(N46-50))), "" )</f>
         <v/>
       </c>
       <c r="H46">
@@ -3126,7 +3171,7 @@
         <v>1</v>
       </c>
       <c r="N46">
-        <f t="shared" si="4"/>
+        <f>IF((H46+I46+J46+L46+M46+O46)&lt;70,IF((H46+I46+J46+L46+M46+O46)&gt;59,70,(H46+I46+J46+L46+M46+O46)),(H46+I46+J46+L46+M46+O46))</f>
         <v>38</v>
       </c>
     </row>
@@ -3141,19 +3186,19 @@
         <v>105</v>
       </c>
       <c r="D47" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N47)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E47" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N47)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F47" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N47)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G47" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N47)&gt;=70,IF((N47-50)&gt;50,50,IF((N47-50)&lt;0,0,(N47-50))), "" )</f>
         <v/>
       </c>
       <c r="J47">
@@ -3162,9 +3207,12 @@
       <c r="K47">
         <v>1</v>
       </c>
+      <c r="M47">
+        <v>30</v>
+      </c>
       <c r="N47">
-        <f t="shared" si="4"/>
-        <v>16</v>
+        <f>IF((H47+I47+J47+L47+M47+O47)&lt;70,IF((H47+I47+J47+L47+M47+O47)&gt;59,70,(H47+I47+J47+L47+M47+O47)),(H47+I47+J47+L47+M47+O47))</f>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3178,19 +3226,19 @@
         <v>107</v>
       </c>
       <c r="D48" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N48)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E48" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N48)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F48" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N48)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G48" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N48)&gt;=70,IF((N48-50)&gt;50,50,IF((N48-50)&lt;0,0,(N48-50))), "" )</f>
         <v/>
       </c>
       <c r="J48">
@@ -3200,7 +3248,7 @@
         <v>1</v>
       </c>
       <c r="N48">
-        <f t="shared" si="4"/>
+        <f>IF((H48+I48+J48+L48+M48+O48)&lt;70,IF((H48+I48+J48+L48+M48+O48)&gt;59,70,(H48+I48+J48+L48+M48+O48)),(H48+I48+J48+L48+M48+O48))</f>
         <v>14</v>
       </c>
     </row>
@@ -3215,19 +3263,19 @@
         <v>109</v>
       </c>
       <c r="D49" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N49)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E49" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N49)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F49" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N49)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G49" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N49)&gt;=70,IF((N49-50)&gt;50,50,IF((N49-50)&lt;0,0,(N49-50))), "" )</f>
         <v/>
       </c>
       <c r="H49">
@@ -3240,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="N49">
-        <f t="shared" si="4"/>
+        <f>IF((H49+I49+J49+L49+M49+O49)&lt;70,IF((H49+I49+J49+L49+M49+O49)&gt;59,70,(H49+I49+J49+L49+M49+O49)),(H49+I49+J49+L49+M49+O49))</f>
         <v>25</v>
       </c>
     </row>
@@ -3255,26 +3303,26 @@
         <v>111</v>
       </c>
       <c r="D50" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N50)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E50" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N50)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F50" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N50)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G50" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N50)&gt;=70,IF((N50-50)&gt;50,50,IF((N50-50)&lt;0,0,(N50-50))), "" )</f>
         <v/>
       </c>
       <c r="K50">
         <v>1</v>
       </c>
       <c r="N50">
-        <f t="shared" si="4"/>
+        <f>IF((H50+I50+J50+L50+M50+O50)&lt;70,IF((H50+I50+J50+L50+M50+O50)&gt;59,70,(H50+I50+J50+L50+M50+O50)),(H50+I50+J50+L50+M50+O50))</f>
         <v>0</v>
       </c>
     </row>
@@ -3289,26 +3337,26 @@
         <v>113</v>
       </c>
       <c r="D51" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N51)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E51" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N51)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F51" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N51)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G51" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N51)&gt;=70,IF((N51-50)&gt;50,50,IF((N51-50)&lt;0,0,(N51-50))), "" )</f>
         <v/>
       </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="N51">
-        <f t="shared" si="4"/>
+        <f>IF((H51+I51+J51+L51+M51+O51)&lt;70,IF((H51+I51+J51+L51+M51+O51)&gt;59,70,(H51+I51+J51+L51+M51+O51)),(H51+I51+J51+L51+M51+O51))</f>
         <v>0</v>
       </c>
     </row>
@@ -3323,19 +3371,19 @@
         <v>115</v>
       </c>
       <c r="D52" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N52)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N52)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N52)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G52" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N52)&gt;=70,IF((N52-50)&gt;50,50,IF((N52-50)&lt;0,0,(N52-50))), "" )</f>
         <v>38</v>
       </c>
       <c r="H52">
@@ -3357,7 +3405,7 @@
         <v>30</v>
       </c>
       <c r="N52">
-        <f t="shared" si="4"/>
+        <f>IF((H52+I52+J52+L52+M52+O52)&lt;70,IF((H52+I52+J52+L52+M52+O52)&gt;59,70,(H52+I52+J52+L52+M52+O52)),(H52+I52+J52+L52+M52+O52))</f>
         <v>88</v>
       </c>
     </row>
@@ -3371,21 +3419,21 @@
       <c r="C53" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E53" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F53" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G53" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D53" s="6">
+        <f>IF((N53)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E53" s="2">
+        <f>IF((N53)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F53" s="2">
+        <f>IF((N53)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G53" s="6">
+        <f>IF((N53)&gt;=70,IF((N53-50)&gt;50,50,IF((N53-50)&lt;0,0,(N53-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H53">
         <v>17</v>
@@ -3399,9 +3447,12 @@
       <c r="L53">
         <v>18</v>
       </c>
+      <c r="M53">
+        <v>15</v>
+      </c>
       <c r="N53">
-        <f t="shared" si="4"/>
-        <v>55</v>
+        <f>IF((H53+I53+J53+L53+M53+O53)&lt;70,IF((H53+I53+J53+L53+M53+O53)&gt;59,70,(H53+I53+J53+L53+M53+O53)),(H53+I53+J53+L53+M53+O53))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3415,19 +3466,19 @@
         <v>119</v>
       </c>
       <c r="D54" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N54)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N54)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N54)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G54" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N54)&gt;=70,IF((N54-50)&gt;50,50,IF((N54-50)&lt;0,0,(N54-50))), "" )</f>
         <v>42</v>
       </c>
       <c r="H54">
@@ -3449,7 +3500,7 @@
         <v>30</v>
       </c>
       <c r="N54">
-        <f t="shared" si="4"/>
+        <f>IF((H54+I54+J54+L54+M54+O54)&lt;70,IF((H54+I54+J54+L54+M54+O54)&gt;59,70,(H54+I54+J54+L54+M54+O54)),(H54+I54+J54+L54+M54+O54))</f>
         <v>92</v>
       </c>
     </row>
@@ -3463,21 +3514,21 @@
       <c r="C55" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E55" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F55" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G55" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D55" s="6">
+        <f>IF((N55)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E55" s="2">
+        <f>IF((N55)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F55" s="2">
+        <f>IF((N55)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G55" s="6">
+        <f>IF((N55)&gt;=70,IF((N55-50)&gt;50,50,IF((N55-50)&lt;0,0,(N55-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H55">
         <v>12</v>
@@ -3491,9 +3542,12 @@
       <c r="L55">
         <v>18</v>
       </c>
+      <c r="M55">
+        <v>12</v>
+      </c>
       <c r="N55">
-        <f t="shared" si="4"/>
-        <v>48</v>
+        <f>IF((H55+I55+J55+L55+M55+O55)&lt;70,IF((H55+I55+J55+L55+M55+O55)&gt;59,70,(H55+I55+J55+L55+M55+O55)),(H55+I55+J55+L55+M55+O55))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3507,19 +3561,19 @@
         <v>123</v>
       </c>
       <c r="D56" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N56)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N56)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N56)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G56" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N56)&gt;=70,IF((N56-50)&gt;50,50,IF((N56-50)&lt;0,0,(N56-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H56">
@@ -3535,7 +3589,7 @@
         <v>30</v>
       </c>
       <c r="N56">
-        <f t="shared" si="4"/>
+        <f>IF((H56+I56+J56+L56+M56+O56)&lt;70,IF((H56+I56+J56+L56+M56+O56)&gt;59,70,(H56+I56+J56+L56+M56+O56)),(H56+I56+J56+L56+M56+O56))</f>
         <v>70</v>
       </c>
     </row>
@@ -3550,26 +3604,26 @@
         <v>125</v>
       </c>
       <c r="D57" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N57)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E57" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N57)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F57" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N57)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G57" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N57)&gt;=70,IF((N57-50)&gt;50,50,IF((N57-50)&lt;0,0,(N57-50))), "" )</f>
         <v/>
       </c>
       <c r="K57">
         <v>1</v>
       </c>
       <c r="N57">
-        <f t="shared" si="4"/>
+        <f>IF((H57+I57+J57+L57+M57+O57)&lt;70,IF((H57+I57+J57+L57+M57+O57)&gt;59,70,(H57+I57+J57+L57+M57+O57)),(H57+I57+J57+L57+M57+O57))</f>
         <v>0</v>
       </c>
     </row>
@@ -3584,19 +3638,19 @@
         <v>127</v>
       </c>
       <c r="D58" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N58)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E58" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N58)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F58" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N58)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G58" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N58)&gt;=70,IF((N58-50)&gt;50,50,IF((N58-50)&lt;0,0,(N58-50))), "" )</f>
         <v/>
       </c>
       <c r="J58">
@@ -3606,7 +3660,7 @@
         <v>1</v>
       </c>
       <c r="N58">
-        <f t="shared" si="4"/>
+        <f>IF((H58+I58+J58+L58+M58+O58)&lt;70,IF((H58+I58+J58+L58+M58+O58)&gt;59,70,(H58+I58+J58+L58+M58+O58)),(H58+I58+J58+L58+M58+O58))</f>
         <v>10</v>
       </c>
     </row>
@@ -3621,20 +3675,20 @@
         <v>129</v>
       </c>
       <c r="D59" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N59)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N59)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F59" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N59)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G59" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N59)&gt;=70,IF((N59-50)&gt;50,50,IF((N59-50)&lt;0,0,(N59-50))), "" )</f>
+        <v>39</v>
       </c>
       <c r="H59">
         <v>18</v>
@@ -3651,9 +3705,12 @@
       <c r="L59">
         <v>15</v>
       </c>
+      <c r="M59">
+        <v>28</v>
+      </c>
       <c r="N59">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H59+I59+J59+L59+M59+O59)&lt;70,IF((H59+I59+J59+L59+M59+O59)&gt;59,70,(H59+I59+J59+L59+M59+O59)),(H59+I59+J59+L59+M59+O59))</f>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3666,21 +3723,21 @@
       <c r="C60" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E60" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F60" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G60" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D60" s="6">
+        <f>IF((N60)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E60" s="2">
+        <f>IF((N60)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F60" s="2">
+        <f>IF((N60)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G60" s="6">
+        <f>IF((N60)&gt;=70,IF((N60-50)&gt;50,50,IF((N60-50)&lt;0,0,(N60-50))), "" )</f>
+        <v>36</v>
       </c>
       <c r="H60">
         <v>16</v>
@@ -3697,9 +3754,12 @@
       <c r="L60">
         <v>16</v>
       </c>
+      <c r="M60">
+        <v>27</v>
+      </c>
       <c r="N60">
-        <f t="shared" si="4"/>
-        <v>59</v>
+        <f>IF((H60+I60+J60+L60+M60+O60)&lt;70,IF((H60+I60+J60+L60+M60+O60)&gt;59,70,(H60+I60+J60+L60+M60+O60)),(H60+I60+J60+L60+M60+O60))</f>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3712,21 +3772,21 @@
       <c r="C61" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E61" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F61" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G61" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D61" s="6">
+        <f>IF((N61)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E61" s="2">
+        <f>IF((N61)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F61" s="2">
+        <f>IF((N61)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G61" s="6">
+        <f>IF((N61)&gt;=70,IF((N61-50)&gt;50,50,IF((N61-50)&lt;0,0,(N61-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H61">
         <v>17</v>
@@ -3743,9 +3803,12 @@
       <c r="L61">
         <v>16</v>
       </c>
+      <c r="M61">
+        <v>3</v>
+      </c>
       <c r="N61">
-        <f t="shared" si="4"/>
-        <v>57</v>
+        <f>IF((H61+I61+J61+L61+M61+O61)&lt;70,IF((H61+I61+J61+L61+M61+O61)&gt;59,70,(H61+I61+J61+L61+M61+O61)),(H61+I61+J61+L61+M61+O61))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3759,19 +3822,19 @@
         <v>135</v>
       </c>
       <c r="D62" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N62)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N62)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F62" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N62)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G62" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N62)&gt;=70,IF((N62-50)&gt;50,50,IF((N62-50)&lt;0,0,(N62-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H62">
@@ -3790,7 +3853,7 @@
         <v>20</v>
       </c>
       <c r="N62">
-        <f t="shared" si="4"/>
+        <f>IF((H62+I62+J62+L62+M62+O62)&lt;70,IF((H62+I62+J62+L62+M62+O62)&gt;59,70,(H62+I62+J62+L62+M62+O62)),(H62+I62+J62+L62+M62+O62))</f>
         <v>70</v>
       </c>
     </row>
@@ -3805,19 +3868,19 @@
         <v>137</v>
       </c>
       <c r="D63" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N63)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N63)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F63" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N63)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G63" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N63)&gt;=70,IF((N63-50)&gt;50,50,IF((N63-50)&lt;0,0,(N63-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H63">
@@ -3836,7 +3899,7 @@
         <v>16</v>
       </c>
       <c r="N63">
-        <f t="shared" si="4"/>
+        <f>IF((H63+I63+J63+L63+M63+O63)&lt;70,IF((H63+I63+J63+L63+M63+O63)&gt;59,70,(H63+I63+J63+L63+M63+O63)),(H63+I63+J63+L63+M63+O63))</f>
         <v>70</v>
       </c>
     </row>
@@ -3851,20 +3914,20 @@
         <v>139</v>
       </c>
       <c r="D64" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N64)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N64)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F64" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N64)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G64" s="6">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>IF((N64)&gt;=70,IF((N64-50)&gt;50,50,IF((N64-50)&lt;0,0,(N64-50))), "" )</f>
+        <v>39</v>
       </c>
       <c r="H64">
         <v>16</v>
@@ -3881,9 +3944,12 @@
       <c r="L64">
         <v>19</v>
       </c>
+      <c r="M64">
+        <v>27</v>
+      </c>
       <c r="N64">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f>IF((H64+I64+J64+L64+M64+O64)&lt;70,IF((H64+I64+J64+L64+M64+O64)&gt;59,70,(H64+I64+J64+L64+M64+O64)),(H64+I64+J64+L64+M64+O64))</f>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3897,19 +3963,19 @@
         <v>141</v>
       </c>
       <c r="D65" s="6">
-        <f t="shared" si="0"/>
+        <f>IF((N65)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E65" s="2">
-        <f t="shared" si="1"/>
+        <f>IF((N65)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F65" s="2">
-        <f t="shared" si="2"/>
+        <f>IF((N65)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G65" s="6">
-        <f t="shared" si="3"/>
+        <f>IF((N65)&gt;=70,IF((N65-50)&gt;50,50,IF((N65-50)&lt;0,0,(N65-50))), "" )</f>
         <v>26</v>
       </c>
       <c r="H65">
@@ -3931,7 +3997,7 @@
         <v>30</v>
       </c>
       <c r="N65">
-        <f t="shared" si="4"/>
+        <f>IF((H65+I65+J65+L65+M65+O65)&lt;70,IF((H65+I65+J65+L65+M65+O65)&gt;59,70,(H65+I65+J65+L65+M65+O65)),(H65+I65+J65+L65+M65+O65))</f>
         <v>76</v>
       </c>
     </row>
@@ -3946,19 +4012,19 @@
         <v>143</v>
       </c>
       <c r="D66" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF((N66)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E66" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF((N66)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F66" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>IF((N66)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G66" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f>IF((N66)&gt;=70,IF((N66-50)&gt;50,50,IF((N66-50)&lt;0,0,(N66-50))), "" )</f>
         <v/>
       </c>
       <c r="H66">
@@ -3970,9 +4036,12 @@
       <c r="K66">
         <v>1</v>
       </c>
+      <c r="M66">
+        <v>15</v>
+      </c>
       <c r="N66">
-        <f t="shared" si="4"/>
-        <v>34</v>
+        <f>IF((H66+I66+J66+L66+M66+O66)&lt;70,IF((H66+I66+J66+L66+M66+O66)&gt;59,70,(H66+I66+J66+L66+M66+O66)),(H66+I66+J66+L66+M66+O66))</f>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3986,19 +4055,19 @@
         <v>145</v>
       </c>
       <c r="D67" s="6">
-        <f t="shared" ref="D67:D90" si="5">IF((N67)&gt;=70,10,"")</f>
+        <f>IF((N67)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E67" s="2">
-        <f t="shared" ref="E67:E90" si="6">IF((N67)&gt;=70,20,"")</f>
+        <f>IF((N67)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F67" s="2">
-        <f t="shared" ref="F67:F90" si="7">IF((N67)&gt;=70,20,"")</f>
+        <f>IF((N67)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G67" s="6">
-        <f t="shared" ref="G67:G90" si="8">IF((N67)&gt;=70,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
+        <f>IF((N67)&gt;=70,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
         <v>29</v>
       </c>
       <c r="H67">
@@ -4017,7 +4086,7 @@
         <v>27</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N90" si="9">IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
+        <f>IF((H67+I67+J67+L67+M67+O67)&lt;70,IF((H67+I67+J67+L67+M67+O67)&gt;59,70,(H67+I67+J67+L67+M67+O67)),(H67+I67+J67+L67+M67+O67))</f>
         <v>79</v>
       </c>
     </row>
@@ -4032,19 +4101,19 @@
         <v>147</v>
       </c>
       <c r="D68" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N68)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E68" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N68)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F68" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N68)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G68" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N68)&gt;=70,IF((N68-50)&gt;50,50,IF((N68-50)&lt;0,0,(N68-50))), "" )</f>
         <v>26</v>
       </c>
       <c r="H68">
@@ -4063,7 +4132,7 @@
         <v>23</v>
       </c>
       <c r="N68">
-        <f t="shared" si="9"/>
+        <f>IF((H68+I68+J68+L68+M68+O68)&lt;70,IF((H68+I68+J68+L68+M68+O68)&gt;59,70,(H68+I68+J68+L68+M68+O68)),(H68+I68+J68+L68+M68+O68))</f>
         <v>76</v>
       </c>
     </row>
@@ -4078,19 +4147,19 @@
         <v>149</v>
       </c>
       <c r="D69" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N69)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E69" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N69)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F69" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N69)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G69" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N69)&gt;=70,IF((N69-50)&gt;50,50,IF((N69-50)&lt;0,0,(N69-50))), "" )</f>
         <v/>
       </c>
       <c r="J69">
@@ -4100,7 +4169,7 @@
         <v>1</v>
       </c>
       <c r="N69">
-        <f t="shared" si="9"/>
+        <f>IF((H69+I69+J69+L69+M69+O69)&lt;70,IF((H69+I69+J69+L69+M69+O69)&gt;59,70,(H69+I69+J69+L69+M69+O69)),(H69+I69+J69+L69+M69+O69))</f>
         <v>18</v>
       </c>
     </row>
@@ -4115,19 +4184,19 @@
         <v>151</v>
       </c>
       <c r="D70" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N70)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E70" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N70)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F70" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N70)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G70" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N70)&gt;=70,IF((N70-50)&gt;50,50,IF((N70-50)&lt;0,0,(N70-50))), "" )</f>
         <v>31</v>
       </c>
       <c r="H70">
@@ -4146,7 +4215,7 @@
         <v>29</v>
       </c>
       <c r="N70">
-        <f t="shared" si="9"/>
+        <f>IF((H70+I70+J70+L70+M70+O70)&lt;70,IF((H70+I70+J70+L70+M70+O70)&gt;59,70,(H70+I70+J70+L70+M70+O70)),(H70+I70+J70+L70+M70+O70))</f>
         <v>81</v>
       </c>
     </row>
@@ -4161,19 +4230,19 @@
         <v>153</v>
       </c>
       <c r="D71" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N71)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E71" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N71)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F71" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N71)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G71" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N71)&gt;=70,IF((N71-50)&gt;50,50,IF((N71-50)&lt;0,0,(N71-50))), "" )</f>
         <v>39</v>
       </c>
       <c r="H71">
@@ -4195,7 +4264,7 @@
         <v>27</v>
       </c>
       <c r="N71">
-        <f t="shared" si="9"/>
+        <f>IF((H71+I71+J71+L71+M71+O71)&lt;70,IF((H71+I71+J71+L71+M71+O71)&gt;59,70,(H71+I71+J71+L71+M71+O71)),(H71+I71+J71+L71+M71+O71))</f>
         <v>89</v>
       </c>
     </row>
@@ -4210,19 +4279,19 @@
         <v>155</v>
       </c>
       <c r="D72" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N72)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E72" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N72)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F72" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N72)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G72" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N72)&gt;=70,IF((N72-50)&gt;50,50,IF((N72-50)&lt;0,0,(N72-50))), "" )</f>
         <v>20</v>
       </c>
       <c r="H72">
@@ -4242,7 +4311,7 @@
         <v>20</v>
       </c>
       <c r="N72">
-        <f t="shared" si="9"/>
+        <f>IF((H72+I72+J72+L72+M72+O72)&lt;70,IF((H72+I72+J72+L72+M72+O72)&gt;59,70,(H72+I72+J72+L72+M72+O72)),(H72+I72+J72+L72+M72+O72))</f>
         <v>70</v>
       </c>
     </row>
@@ -4257,19 +4326,19 @@
         <v>157</v>
       </c>
       <c r="D73" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N73)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E73" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N73)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F73" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N73)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G73" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N73)&gt;=70,IF((N73-50)&gt;50,50,IF((N73-50)&lt;0,0,(N73-50))), "" )</f>
         <v/>
       </c>
       <c r="H73">
@@ -4281,9 +4350,12 @@
       <c r="K73">
         <v>1</v>
       </c>
+      <c r="M73">
+        <v>29</v>
+      </c>
       <c r="N73">
-        <f t="shared" si="9"/>
-        <v>26</v>
+        <f>IF((H73+I73+J73+L73+M73+O73)&lt;70,IF((H73+I73+J73+L73+M73+O73)&gt;59,70,(H73+I73+J73+L73+M73+O73)),(H73+I73+J73+L73+M73+O73))</f>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4297,20 +4369,20 @@
         <v>159</v>
       </c>
       <c r="D74" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N74)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E74" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N74)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F74" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N74)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G74" s="6">
-        <f t="shared" si="8"/>
-        <v>20</v>
+        <f>IF((N74)&gt;=70,IF((N74-50)&gt;50,50,IF((N74-50)&lt;0,0,(N74-50))), "" )</f>
+        <v>44</v>
       </c>
       <c r="H74">
         <v>18</v>
@@ -4327,9 +4399,12 @@
       <c r="L74">
         <v>18</v>
       </c>
+      <c r="M74">
+        <v>28</v>
+      </c>
       <c r="N74">
-        <f t="shared" si="9"/>
-        <v>70</v>
+        <f>IF((H74+I74+J74+L74+M74+O74)&lt;70,IF((H74+I74+J74+L74+M74+O74)&gt;59,70,(H74+I74+J74+L74+M74+O74)),(H74+I74+J74+L74+M74+O74))</f>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4343,19 +4418,19 @@
         <v>161</v>
       </c>
       <c r="D75" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N75)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E75" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N75)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F75" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N75)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G75" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N75)&gt;=70,IF((N75-50)&gt;50,50,IF((N75-50)&lt;0,0,(N75-50))), "" )</f>
         <v>46</v>
       </c>
       <c r="H75">
@@ -4377,7 +4452,7 @@
         <v>30</v>
       </c>
       <c r="N75">
-        <f t="shared" si="9"/>
+        <f>IF((H75+I75+J75+L75+M75+O75)&lt;70,IF((H75+I75+J75+L75+M75+O75)&gt;59,70,(H75+I75+J75+L75+M75+O75)),(H75+I75+J75+L75+M75+O75))</f>
         <v>96</v>
       </c>
     </row>
@@ -4391,21 +4466,21 @@
       <c r="C76" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D76" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E76" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F76" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G76" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D76" s="6">
+        <f>IF((N76)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E76" s="2">
+        <f>IF((N76)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F76" s="2">
+        <f>IF((N76)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G76" s="6">
+        <f>IF((N76)&gt;=70,IF((N76-50)&gt;50,50,IF((N76-50)&lt;0,0,(N76-50))), "" )</f>
+        <v>25</v>
       </c>
       <c r="H76">
         <v>16</v>
@@ -4419,9 +4494,12 @@
       <c r="L76">
         <v>15</v>
       </c>
+      <c r="M76">
+        <v>27</v>
+      </c>
       <c r="N76">
-        <f t="shared" si="9"/>
-        <v>48</v>
+        <f>IF((H76+I76+J76+L76+M76+O76)&lt;70,IF((H76+I76+J76+L76+M76+O76)&gt;59,70,(H76+I76+J76+L76+M76+O76)),(H76+I76+J76+L76+M76+O76))</f>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4435,26 +4513,26 @@
         <v>165</v>
       </c>
       <c r="D77" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f>IF((N77)&gt;=70,10,"")</f>
         <v/>
       </c>
       <c r="E77" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f>IF((N77)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="F77" s="2" t="str">
-        <f t="shared" si="7"/>
+        <f>IF((N77)&gt;=70,20,"")</f>
         <v/>
       </c>
       <c r="G77" s="6" t="str">
-        <f t="shared" si="8"/>
+        <f>IF((N77)&gt;=70,IF((N77-50)&gt;50,50,IF((N77-50)&lt;0,0,(N77-50))), "" )</f>
         <v/>
       </c>
       <c r="K77">
         <v>1</v>
       </c>
       <c r="N77">
-        <f t="shared" si="9"/>
+        <f>IF((H77+I77+J77+L77+M77+O77)&lt;70,IF((H77+I77+J77+L77+M77+O77)&gt;59,70,(H77+I77+J77+L77+M77+O77)),(H77+I77+J77+L77+M77+O77))</f>
         <v>0</v>
       </c>
     </row>
@@ -4469,19 +4547,19 @@
         <v>167</v>
       </c>
       <c r="D78" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N78)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E78" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N78)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F78" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N78)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G78" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N78)&gt;=70,IF((N78-50)&gt;50,50,IF((N78-50)&lt;0,0,(N78-50))), "" )</f>
         <v>42</v>
       </c>
       <c r="H78">
@@ -4503,7 +4581,7 @@
         <v>30</v>
       </c>
       <c r="N78">
-        <f t="shared" si="9"/>
+        <f>IF((H78+I78+J78+L78+M78+O78)&lt;70,IF((H78+I78+J78+L78+M78+O78)&gt;59,70,(H78+I78+J78+L78+M78+O78)),(H78+I78+J78+L78+M78+O78))</f>
         <v>92</v>
       </c>
     </row>
@@ -4518,19 +4596,19 @@
         <v>169</v>
       </c>
       <c r="D79" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N79)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E79" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N79)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F79" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N79)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G79" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N79)&gt;=70,IF((N79-50)&gt;50,50,IF((N79-50)&lt;0,0,(N79-50))), "" )</f>
         <v>35</v>
       </c>
       <c r="H79">
@@ -4549,7 +4627,7 @@
         <v>30</v>
       </c>
       <c r="N79">
-        <f t="shared" si="9"/>
+        <f>IF((H79+I79+J79+L79+M79+O79)&lt;70,IF((H79+I79+J79+L79+M79+O79)&gt;59,70,(H79+I79+J79+L79+M79+O79)),(H79+I79+J79+L79+M79+O79))</f>
         <v>85</v>
       </c>
     </row>
@@ -4564,19 +4642,19 @@
         <v>171</v>
       </c>
       <c r="D80" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N80)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E80" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N80)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F80" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N80)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G80" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N80)&gt;=70,IF((N80-50)&gt;50,50,IF((N80-50)&lt;0,0,(N80-50))), "" )</f>
         <v>43</v>
       </c>
       <c r="H80">
@@ -4598,7 +4676,7 @@
         <v>30</v>
       </c>
       <c r="N80">
-        <f t="shared" si="9"/>
+        <f>IF((H80+I80+J80+L80+M80+O80)&lt;70,IF((H80+I80+J80+L80+M80+O80)&gt;59,70,(H80+I80+J80+L80+M80+O80)),(H80+I80+J80+L80+M80+O80))</f>
         <v>93</v>
       </c>
     </row>
@@ -4613,19 +4691,19 @@
         <v>173</v>
       </c>
       <c r="D81" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N81)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E81" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N81)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F81" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N81)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G81" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N81)&gt;=70,IF((N81-50)&gt;50,50,IF((N81-50)&lt;0,0,(N81-50))), "" )</f>
         <v>27</v>
       </c>
       <c r="H81">
@@ -4644,7 +4722,7 @@
         <v>30</v>
       </c>
       <c r="N81">
-        <f t="shared" si="9"/>
+        <f>IF((H81+I81+J81+L81+M81+O81)&lt;70,IF((H81+I81+J81+L81+M81+O81)&gt;59,70,(H81+I81+J81+L81+M81+O81)),(H81+I81+J81+L81+M81+O81))</f>
         <v>77</v>
       </c>
     </row>
@@ -4659,19 +4737,19 @@
         <v>175</v>
       </c>
       <c r="D82" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N82)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E82" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N82)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F82" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N82)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G82" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N82)&gt;=70,IF((N82-50)&gt;50,50,IF((N82-50)&lt;0,0,(N82-50))), "" )</f>
         <v>32</v>
       </c>
       <c r="H82">
@@ -4690,7 +4768,7 @@
         <v>30</v>
       </c>
       <c r="N82">
-        <f t="shared" si="9"/>
+        <f>IF((H82+I82+J82+L82+M82+O82)&lt;70,IF((H82+I82+J82+L82+M82+O82)&gt;59,70,(H82+I82+J82+L82+M82+O82)),(H82+I82+J82+L82+M82+O82))</f>
         <v>82</v>
       </c>
     </row>
@@ -4705,19 +4783,19 @@
         <v>177</v>
       </c>
       <c r="D83" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N83)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E83" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N83)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F83" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N83)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G83" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N83)&gt;=70,IF((N83-50)&gt;50,50,IF((N83-50)&lt;0,0,(N83-50))), "" )</f>
         <v>44</v>
       </c>
       <c r="H83">
@@ -4739,7 +4817,7 @@
         <v>28</v>
       </c>
       <c r="N83">
-        <f t="shared" si="9"/>
+        <f>IF((H83+I83+J83+L83+M83+O83)&lt;70,IF((H83+I83+J83+L83+M83+O83)&gt;59,70,(H83+I83+J83+L83+M83+O83)),(H83+I83+J83+L83+M83+O83))</f>
         <v>94</v>
       </c>
     </row>
@@ -4753,21 +4831,21 @@
       <c r="C84" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="D84" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E84" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F84" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G84" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D84" s="6">
+        <f>IF((N84)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E84" s="2">
+        <f>IF((N84)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F84" s="2">
+        <f>IF((N84)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G84" s="6">
+        <f>IF((N84)&gt;=70,IF((N84-50)&gt;50,50,IF((N84-50)&lt;0,0,(N84-50))), "" )</f>
+        <v>21</v>
       </c>
       <c r="H84">
         <v>16</v>
@@ -4781,9 +4859,12 @@
       <c r="L84">
         <v>18</v>
       </c>
+      <c r="M84">
+        <v>20</v>
+      </c>
       <c r="N84">
-        <f t="shared" si="9"/>
-        <v>51</v>
+        <f>IF((H84+I84+J84+L84+M84+O84)&lt;70,IF((H84+I84+J84+L84+M84+O84)&gt;59,70,(H84+I84+J84+L84+M84+O84)),(H84+I84+J84+L84+M84+O84))</f>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4797,19 +4878,19 @@
         <v>181</v>
       </c>
       <c r="D85" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N85)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E85" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N85)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F85" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N85)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G85" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N85)&gt;=70,IF((N85-50)&gt;50,50,IF((N85-50)&lt;0,0,(N85-50))), "" )</f>
         <v>43</v>
       </c>
       <c r="H85">
@@ -4831,7 +4912,7 @@
         <v>29</v>
       </c>
       <c r="N85">
-        <f t="shared" si="9"/>
+        <f>IF((H85+I85+J85+L85+M85+O85)&lt;70,IF((H85+I85+J85+L85+M85+O85)&gt;59,70,(H85+I85+J85+L85+M85+O85)),(H85+I85+J85+L85+M85+O85))</f>
         <v>93</v>
       </c>
     </row>
@@ -4846,19 +4927,19 @@
         <v>183</v>
       </c>
       <c r="D86" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N86)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E86" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N86)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F86" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N86)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G86" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N86)&gt;=70,IF((N86-50)&gt;50,50,IF((N86-50)&lt;0,0,(N86-50))), "" )</f>
         <v>44</v>
       </c>
       <c r="H86">
@@ -4880,7 +4961,7 @@
         <v>28</v>
       </c>
       <c r="N86">
-        <f t="shared" si="9"/>
+        <f>IF((H86+I86+J86+L86+M86+O86)&lt;70,IF((H86+I86+J86+L86+M86+O86)&gt;59,70,(H86+I86+J86+L86+M86+O86)),(H86+I86+J86+L86+M86+O86))</f>
         <v>94</v>
       </c>
     </row>
@@ -4895,19 +4976,19 @@
         <v>185</v>
       </c>
       <c r="D87" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N87)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E87" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N87)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F87" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N87)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G87" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N87)&gt;=70,IF((N87-50)&gt;50,50,IF((N87-50)&lt;0,0,(N87-50))), "" )</f>
         <v>31</v>
       </c>
       <c r="H87">
@@ -4926,7 +5007,7 @@
         <v>28</v>
       </c>
       <c r="N87">
-        <f t="shared" si="9"/>
+        <f>IF((H87+I87+J87+L87+M87+O87)&lt;70,IF((H87+I87+J87+L87+M87+O87)&gt;59,70,(H87+I87+J87+L87+M87+O87)),(H87+I87+J87+L87+M87+O87))</f>
         <v>81</v>
       </c>
     </row>
@@ -4940,21 +5021,21 @@
       <c r="C88" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="D88" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E88" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F88" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G88" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D88" s="6">
+        <f>IF((N88)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E88" s="2">
+        <f>IF((N88)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F88" s="2">
+        <f>IF((N88)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G88" s="6">
+        <f>IF((N88)&gt;=70,IF((N88-50)&gt;50,50,IF((N88-50)&lt;0,0,(N88-50))), "" )</f>
+        <v>24</v>
       </c>
       <c r="H88">
         <v>18</v>
@@ -4968,9 +5049,12 @@
       <c r="K88">
         <v>2</v>
       </c>
+      <c r="M88">
+        <v>28</v>
+      </c>
       <c r="N88">
-        <f t="shared" si="9"/>
-        <v>46</v>
+        <f>IF((H88+I88+J88+L88+M88+O88)&lt;70,IF((H88+I88+J88+L88+M88+O88)&gt;59,70,(H88+I88+J88+L88+M88+O88)),(H88+I88+J88+L88+M88+O88))</f>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -4983,21 +5067,21 @@
       <c r="C89" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="D89" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E89" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F89" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G89" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v/>
+      <c r="D89" s="6">
+        <f>IF((N89)&gt;=70,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E89" s="2">
+        <f>IF((N89)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F89" s="2">
+        <f>IF((N89)&gt;=70,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G89" s="6">
+        <f>IF((N89)&gt;=70,IF((N89-50)&gt;50,50,IF((N89-50)&lt;0,0,(N89-50))), "" )</f>
+        <v>20</v>
       </c>
       <c r="H89">
         <v>16</v>
@@ -5011,9 +5095,12 @@
       <c r="L89">
         <v>20</v>
       </c>
+      <c r="M89">
+        <v>8</v>
+      </c>
       <c r="N89">
-        <f t="shared" si="9"/>
-        <v>52</v>
+        <f>IF((H89+I89+J89+L89+M89+O89)&lt;70,IF((H89+I89+J89+L89+M89+O89)&gt;59,70,(H89+I89+J89+L89+M89+O89)),(H89+I89+J89+L89+M89+O89))</f>
+        <v>70</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -5027,19 +5114,19 @@
         <v>191</v>
       </c>
       <c r="D90" s="6">
-        <f t="shared" si="5"/>
+        <f>IF((N90)&gt;=70,10,"")</f>
         <v>10</v>
       </c>
       <c r="E90" s="2">
-        <f t="shared" si="6"/>
+        <f>IF((N90)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="F90" s="2">
-        <f t="shared" si="7"/>
+        <f>IF((N90)&gt;=70,20,"")</f>
         <v>20</v>
       </c>
       <c r="G90" s="6">
-        <f t="shared" si="8"/>
+        <f>IF((N90)&gt;=70,IF((N90-50)&gt;50,50,IF((N90-50)&lt;0,0,(N90-50))), "" )</f>
         <v>43</v>
       </c>
       <c r="H90">
@@ -5061,16 +5148,19 @@
         <v>29</v>
       </c>
       <c r="N90">
-        <f t="shared" si="9"/>
+        <f>IF((H90+I90+J90+L90+M90+O90)&lt;70,IF((H90+I90+J90+L90+M90+O90)&gt;59,70,(H90+I90+J90+L90+M90+O90)),(H90+I90+J90+L90+M90+O90))</f>
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1">
+  <autoFilter ref="A1:O90">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="6" showButton="0"/>
+    <sortState ref="A2:O90">
+      <sortCondition ref="A1:A90"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.39" right="0.39" top="0.39" bottom="0.39" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>